<commit_message>
Added new soap message for exceptions, added log to track system flow
</commit_message>
<xml_diff>
--- a/doc/messages.xlsx
+++ b/doc/messages.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="158">
   <si>
     <t>Error</t>
   </si>
@@ -478,6 +478,18 @@
   </si>
   <si>
     <t>Shown if an user downloads a dataset which has a duplicate (i.e. another dataset in status different from DELETED with the same sender dataset id exists)</t>
+  </si>
+  <si>
+    <t>Shown if File&gt;download report is pressed and no data collection related to the user was found</t>
+  </si>
+  <si>
+    <t>WARN702</t>
+  </si>
+  <si>
+    <t>ERR104</t>
+  </si>
+  <si>
+    <t>Send message failed as result of SOAP call (probably due to username wrongly typed)</t>
   </si>
 </sst>
 </file>
@@ -569,8 +581,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C63" totalsRowShown="0">
-  <autoFilter ref="A1:C63"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C66" totalsRowShown="0">
+  <autoFilter ref="A1:C66"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Error"/>
     <tableColumn id="2" name="Error code"/>
@@ -892,10 +904,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C63"/>
+  <dimension ref="A1:C66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -962,32 +974,21 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>117</v>
+        <v>157</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>156</v>
       </c>
       <c r="C7" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>118</v>
-      </c>
-      <c r="B8" t="s">
-        <v>116</v>
-      </c>
-      <c r="C8" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>149</v>
+        <v>117</v>
       </c>
       <c r="B9" t="s">
-        <v>146</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
         <v>89</v>
@@ -995,10 +996,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="B10" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="C10" t="s">
         <v>89</v>
@@ -1006,10 +1007,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>149</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>146</v>
       </c>
       <c r="C11" t="s">
         <v>89</v>
@@ -1017,10 +1018,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>129</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>130</v>
       </c>
       <c r="C12" t="s">
         <v>89</v>
@@ -1028,10 +1029,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>80</v>
+        <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="C13" t="s">
         <v>89</v>
@@ -1039,10 +1040,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>125</v>
+        <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>82</v>
+        <v>28</v>
       </c>
       <c r="C14" t="s">
         <v>89</v>
@@ -1050,10 +1051,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="B15" t="s">
-        <v>91</v>
+        <v>48</v>
       </c>
       <c r="C15" t="s">
         <v>89</v>
@@ -1061,10 +1062,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B16" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="C16" t="s">
         <v>89</v>
@@ -1072,10 +1073,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B17" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C17" t="s">
         <v>89</v>
@@ -1083,10 +1084,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>101</v>
+        <v>124</v>
       </c>
       <c r="B18" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="C18" t="s">
         <v>89</v>
@@ -1094,10 +1095,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>42</v>
+        <v>93</v>
       </c>
       <c r="B19" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="C19" t="s">
         <v>89</v>
@@ -1105,10 +1106,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>143</v>
+        <v>101</v>
       </c>
       <c r="B20" t="s">
-        <v>142</v>
+        <v>102</v>
       </c>
       <c r="C20" t="s">
         <v>89</v>
@@ -1116,65 +1117,65 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>144</v>
+        <v>42</v>
       </c>
       <c r="B21" t="s">
-        <v>145</v>
+        <v>114</v>
       </c>
       <c r="C21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>143</v>
+      </c>
+      <c r="B22" t="s">
+        <v>142</v>
+      </c>
+      <c r="C22" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>144</v>
+      </c>
+      <c r="B23" t="s">
+        <v>145</v>
+      </c>
+      <c r="C23" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>71</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B25" t="s">
         <v>43</v>
       </c>
-      <c r="C23" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>150</v>
-      </c>
-      <c r="B24" t="s">
-        <v>151</v>
-      </c>
-      <c r="C24" t="s">
+      <c r="C25" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>27</v>
+        <v>150</v>
       </c>
       <c r="B26" t="s">
-        <v>49</v>
+        <v>151</v>
       </c>
       <c r="C26" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>128</v>
-      </c>
-      <c r="B27" t="s">
-        <v>122</v>
-      </c>
-      <c r="C27" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>109</v>
+        <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>100</v>
+        <v>49</v>
       </c>
       <c r="C28" t="s">
         <v>89</v>
@@ -1182,10 +1183,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B29" t="s">
-        <v>139</v>
+        <v>122</v>
       </c>
       <c r="C29" t="s">
         <v>89</v>
@@ -1193,10 +1194,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>137</v>
+        <v>109</v>
       </c>
       <c r="B30" t="s">
-        <v>138</v>
+        <v>100</v>
       </c>
       <c r="C30" t="s">
         <v>89</v>
@@ -1204,10 +1205,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>141</v>
+        <v>123</v>
       </c>
       <c r="B31" t="s">
-        <v>95</v>
+        <v>139</v>
       </c>
       <c r="C31" t="s">
         <v>89</v>
@@ -1215,10 +1216,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B32" t="s">
-        <v>96</v>
+        <v>138</v>
       </c>
       <c r="C32" t="s">
         <v>89</v>
@@ -1226,10 +1227,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>98</v>
+        <v>141</v>
       </c>
       <c r="B33" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C33" t="s">
         <v>89</v>
@@ -1237,10 +1238,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>121</v>
+        <v>140</v>
       </c>
       <c r="B34" t="s">
-        <v>120</v>
+        <v>96</v>
       </c>
       <c r="C34" t="s">
         <v>89</v>
@@ -1248,10 +1249,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="B35" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="C35" t="s">
         <v>89</v>
@@ -1259,10 +1260,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>147</v>
+        <v>121</v>
       </c>
       <c r="B36" t="s">
-        <v>148</v>
+        <v>120</v>
       </c>
       <c r="C36" t="s">
         <v>89</v>
@@ -1270,10 +1271,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>29</v>
+        <v>105</v>
       </c>
       <c r="B37" t="s">
-        <v>30</v>
+        <v>106</v>
       </c>
       <c r="C37" t="s">
         <v>89</v>
@@ -1281,10 +1282,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>31</v>
+        <v>147</v>
       </c>
       <c r="B38" t="s">
-        <v>32</v>
+        <v>148</v>
       </c>
       <c r="C38" t="s">
         <v>89</v>
@@ -1292,10 +1293,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B39" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C39" t="s">
         <v>89</v>
@@ -1303,10 +1304,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B40" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C40" t="s">
         <v>89</v>
@@ -1314,43 +1315,43 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>62</v>
+        <v>33</v>
       </c>
       <c r="B41" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C41" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>35</v>
+      </c>
+      <c r="B42" t="s">
+        <v>36</v>
+      </c>
+      <c r="C42" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="B43" t="s">
-        <v>83</v>
+        <v>37</v>
       </c>
       <c r="C43" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>38</v>
-      </c>
-      <c r="B44" t="s">
-        <v>44</v>
-      </c>
-      <c r="C44" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>39</v>
+        <v>81</v>
       </c>
       <c r="B45" t="s">
-        <v>45</v>
+        <v>83</v>
       </c>
       <c r="C45" t="s">
         <v>89</v>
@@ -1358,10 +1359,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B46" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C46" t="s">
         <v>89</v>
@@ -1369,98 +1370,98 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B47" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C47" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>40</v>
+      </c>
+      <c r="B48" t="s">
+        <v>46</v>
+      </c>
+      <c r="C48" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>41</v>
+      </c>
+      <c r="B49" t="s">
+        <v>47</v>
+      </c>
+      <c r="C49" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>97</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B51" t="s">
         <v>68</v>
       </c>
-      <c r="C49" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+      <c r="C51" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>70</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B52" t="s">
         <v>69</v>
       </c>
-      <c r="C50" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
+      <c r="C52" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B53" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C51" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
+      <c r="C53" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="B54" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="C52" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>84</v>
-      </c>
-      <c r="B54" t="s">
-        <v>76</v>
-      </c>
       <c r="C54" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>85</v>
-      </c>
-      <c r="B55" t="s">
-        <v>77</v>
+      <c r="A55" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>155</v>
       </c>
       <c r="C55" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>86</v>
-      </c>
-      <c r="B56" t="s">
-        <v>78</v>
-      </c>
-      <c r="C56" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B57" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="C57" t="s">
         <v>89</v>
@@ -1468,10 +1469,10 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>107</v>
+        <v>85</v>
       </c>
       <c r="B58" t="s">
-        <v>108</v>
+        <v>77</v>
       </c>
       <c r="C58" t="s">
         <v>89</v>
@@ -1479,10 +1480,10 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>111</v>
+        <v>86</v>
       </c>
       <c r="B59" t="s">
-        <v>110</v>
+        <v>78</v>
       </c>
       <c r="C59" t="s">
         <v>89</v>
@@ -1490,34 +1491,67 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>112</v>
+        <v>87</v>
       </c>
       <c r="B60" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="C60" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>107</v>
+      </c>
+      <c r="B61" t="s">
+        <v>108</v>
+      </c>
+      <c r="C61" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
+        <v>111</v>
+      </c>
+      <c r="B62" t="s">
+        <v>110</v>
+      </c>
+      <c r="C62" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>112</v>
+      </c>
+      <c r="B63" t="s">
+        <v>79</v>
+      </c>
+      <c r="C63" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>133</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B65" t="s">
         <v>134</v>
       </c>
-      <c r="C62" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
+      <c r="C65" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="B66" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C66" t="s">
         <v>89</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added progress bars for refresh status, display ack and download dataset (get datasets list only).
</commit_message>
<xml_diff>
--- a/doc/messages.xlsx
+++ b/doc/messages.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="164">
   <si>
     <t>Error</t>
   </si>
@@ -489,7 +489,25 @@
     <t>ERR104</t>
   </si>
   <si>
-    <t>Send message failed as result of SOAP call (probably due to username wrongly typed)</t>
+    <t>Send message failed as result of SOAP call (probably due to username wrongly typed or to no connection problems)</t>
+  </si>
+  <si>
+    <t>ERR805</t>
+  </si>
+  <si>
+    <t>Display ack generic error</t>
+  </si>
+  <si>
+    <t>Refresh status generic error</t>
+  </si>
+  <si>
+    <t>ERR503</t>
+  </si>
+  <si>
+    <t>ERR704</t>
+  </si>
+  <si>
+    <t>Generic download report error (get datasets list)</t>
   </si>
 </sst>
 </file>
@@ -581,8 +599,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C66" totalsRowShown="0">
-  <autoFilter ref="A1:C66"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C72" totalsRowShown="0">
+  <autoFilter ref="A1:C72"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Error"/>
     <tableColumn id="2" name="Error code"/>
@@ -904,10 +922,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C66"/>
+  <dimension ref="A1:C72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1170,23 +1188,23 @@
         <v>89</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>27</v>
-      </c>
-      <c r="B28" t="s">
-        <v>49</v>
-      </c>
-      <c r="C28" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>160</v>
+      </c>
+      <c r="B27" t="s">
+        <v>161</v>
+      </c>
+      <c r="C27" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>128</v>
+        <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>122</v>
+        <v>49</v>
       </c>
       <c r="C29" t="s">
         <v>89</v>
@@ -1194,10 +1212,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>109</v>
+        <v>128</v>
       </c>
       <c r="B30" t="s">
-        <v>100</v>
+        <v>122</v>
       </c>
       <c r="C30" t="s">
         <v>89</v>
@@ -1205,10 +1223,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="B31" t="s">
-        <v>139</v>
+        <v>100</v>
       </c>
       <c r="C31" t="s">
         <v>89</v>
@@ -1216,10 +1234,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B32" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C32" t="s">
         <v>89</v>
@@ -1227,10 +1245,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B33" t="s">
-        <v>95</v>
+        <v>138</v>
       </c>
       <c r="C33" t="s">
         <v>89</v>
@@ -1238,32 +1256,21 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>140</v>
+        <v>163</v>
       </c>
       <c r="B34" t="s">
-        <v>96</v>
+        <v>162</v>
       </c>
       <c r="C34" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>98</v>
-      </c>
-      <c r="B35" t="s">
-        <v>99</v>
-      </c>
-      <c r="C35" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>121</v>
+        <v>141</v>
       </c>
       <c r="B36" t="s">
-        <v>120</v>
+        <v>95</v>
       </c>
       <c r="C36" t="s">
         <v>89</v>
@@ -1271,10 +1278,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>105</v>
+        <v>140</v>
       </c>
       <c r="B37" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="C37" t="s">
         <v>89</v>
@@ -1282,10 +1289,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>147</v>
+        <v>98</v>
       </c>
       <c r="B38" t="s">
-        <v>148</v>
+        <v>99</v>
       </c>
       <c r="C38" t="s">
         <v>89</v>
@@ -1293,10 +1300,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>29</v>
+        <v>121</v>
       </c>
       <c r="B39" t="s">
-        <v>30</v>
+        <v>120</v>
       </c>
       <c r="C39" t="s">
         <v>89</v>
@@ -1304,54 +1311,43 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>31</v>
+        <v>159</v>
       </c>
       <c r="B40" t="s">
-        <v>32</v>
+        <v>158</v>
       </c>
       <c r="C40" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>33</v>
-      </c>
-      <c r="B41" t="s">
-        <v>34</v>
-      </c>
-      <c r="C41" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>35</v>
-      </c>
-      <c r="B42" t="s">
-        <v>36</v>
-      </c>
-      <c r="C42" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>62</v>
+        <v>105</v>
       </c>
       <c r="B43" t="s">
-        <v>37</v>
+        <v>106</v>
       </c>
       <c r="C43" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>147</v>
+      </c>
+      <c r="B44" t="s">
+        <v>148</v>
+      </c>
+      <c r="C44" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>81</v>
+        <v>29</v>
       </c>
       <c r="B45" t="s">
-        <v>83</v>
+        <v>30</v>
       </c>
       <c r="C45" t="s">
         <v>89</v>
@@ -1359,10 +1355,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B46" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="C46" t="s">
         <v>89</v>
@@ -1370,10 +1366,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B47" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="C47" t="s">
         <v>89</v>
@@ -1381,10 +1377,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B48" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="C48" t="s">
         <v>89</v>
@@ -1392,10 +1388,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>41</v>
+        <v>62</v>
       </c>
       <c r="B49" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="C49" t="s">
         <v>89</v>
@@ -1403,10 +1399,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="B51" t="s">
-        <v>68</v>
+        <v>83</v>
       </c>
       <c r="C51" t="s">
         <v>89</v>
@@ -1414,43 +1410,43 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>70</v>
+        <v>38</v>
       </c>
       <c r="B52" t="s">
-        <v>69</v>
+        <v>44</v>
       </c>
       <c r="C52" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>67</v>
+      <c r="A53" t="s">
+        <v>39</v>
+      </c>
+      <c r="B53" t="s">
+        <v>45</v>
       </c>
       <c r="C53" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>152</v>
+      <c r="A54" t="s">
+        <v>40</v>
+      </c>
+      <c r="B54" t="s">
+        <v>46</v>
       </c>
       <c r="C54" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>155</v>
+      <c r="A55" t="s">
+        <v>41</v>
+      </c>
+      <c r="B55" t="s">
+        <v>47</v>
       </c>
       <c r="C55" t="s">
         <v>89</v>
@@ -1458,10 +1454,10 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="B57" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="C57" t="s">
         <v>89</v>
@@ -1469,89 +1465,144 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="B58" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="C58" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>86</v>
-      </c>
-      <c r="B59" t="s">
-        <v>78</v>
+      <c r="A59" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="C59" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>87</v>
-      </c>
-      <c r="B60" t="s">
-        <v>88</v>
+      <c r="A60" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>152</v>
       </c>
       <c r="C60" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>107</v>
-      </c>
-      <c r="B61" t="s">
-        <v>108</v>
+      <c r="A61" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>155</v>
       </c>
       <c r="C61" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>111</v>
-      </c>
-      <c r="B62" t="s">
-        <v>110</v>
-      </c>
-      <c r="C62" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>112</v>
+        <v>84</v>
       </c>
       <c r="B63" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C63" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>85</v>
+      </c>
+      <c r="B64" t="s">
+        <v>77</v>
+      </c>
+      <c r="C64" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
+        <v>86</v>
+      </c>
+      <c r="B65" t="s">
+        <v>78</v>
+      </c>
+      <c r="C65" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>87</v>
+      </c>
+      <c r="B66" t="s">
+        <v>88</v>
+      </c>
+      <c r="C66" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>107</v>
+      </c>
+      <c r="B67" t="s">
+        <v>108</v>
+      </c>
+      <c r="C67" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>111</v>
+      </c>
+      <c r="B68" t="s">
+        <v>110</v>
+      </c>
+      <c r="C68" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>112</v>
+      </c>
+      <c r="B69" t="s">
+        <v>79</v>
+      </c>
+      <c r="C69" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
         <v>133</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B71" t="s">
         <v>134</v>
       </c>
-      <c r="C65" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
+      <c r="C71" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="B72" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C72" t="s">
         <v>89</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added junit tests to refresh status
</commit_message>
<xml_diff>
--- a/doc/messages.xlsx
+++ b/doc/messages.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="20010" windowHeight="6240"/>
+    <workbookView xWindow="480" yWindow="165" windowWidth="20010" windowHeight="6180"/>
   </bookViews>
   <sheets>
-    <sheet name="Error codes" sheetId="1" r:id="rId1"/>
-    <sheet name="Error types" sheetId="5" r:id="rId2"/>
+    <sheet name="Message codes" sheetId="1" r:id="rId1"/>
+    <sheet name="Codes descriptions" sheetId="5" r:id="rId2"/>
     <sheet name="Error tests" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="168">
   <si>
     <t>Error</t>
   </si>
@@ -168,9 +168,6 @@
     <t>ERR600</t>
   </si>
   <si>
-    <t>Error type</t>
-  </si>
-  <si>
     <t>1xx</t>
   </si>
   <si>
@@ -213,9 +210,6 @@
     <t>Download report error/warning</t>
   </si>
   <si>
-    <t>Error code group</t>
-  </si>
-  <si>
     <t>Attempt to download a report with the same senderDatasetId of another local report</t>
   </si>
   <si>
@@ -508,6 +502,24 @@
   </si>
   <si>
     <t>Generic download report error (get datasets list)</t>
+  </si>
+  <si>
+    <t>Code group</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>OK500</t>
+  </si>
+  <si>
+    <t>Refresh status successfully completed</t>
+  </si>
+  <si>
+    <t>ERR806</t>
+  </si>
+  <si>
+    <t>Ack is KO, and no errors were found in it =&gt; unknown cause</t>
   </si>
 </sst>
 </file>
@@ -599,8 +611,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C72" totalsRowShown="0">
-  <autoFilter ref="A1:C72"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C78" totalsRowShown="0">
+  <autoFilter ref="A1:C78"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Error"/>
     <tableColumn id="2" name="Error code"/>
@@ -614,8 +626,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:B12" totalsRowShown="0">
   <autoFilter ref="A1:B12"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Error code group"/>
-    <tableColumn id="2" name="Error type"/>
+    <tableColumn id="1" name="Code group"/>
+    <tableColumn id="2" name="Description"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -922,10 +934,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C72"/>
+  <dimension ref="A1:C74"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -943,18 +955,18 @@
         <v>8</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B3" t="s">
         <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -965,7 +977,7 @@
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -976,7 +988,7 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -987,62 +999,62 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B7" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B9" t="s">
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C10" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B11" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B12" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1053,7 +1065,7 @@
         <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1064,73 +1076,73 @@
         <v>28</v>
       </c>
       <c r="C14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B15" t="s">
         <v>48</v>
       </c>
       <c r="C15" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B16" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C16" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B17" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C17" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B18" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C18" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B19" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C19" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B20" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C20" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1138,65 +1150,65 @@
         <v>42</v>
       </c>
       <c r="B21" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B22" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C22" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B23" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C23" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B25" t="s">
         <v>43</v>
       </c>
       <c r="C25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B26" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C26" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B27" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C27" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -1207,139 +1219,150 @@
         <v>49</v>
       </c>
       <c r="C29" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B30" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C30" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B31" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C31" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B32" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C32" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B33" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C33" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B34" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C34" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B36" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C36" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B37" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C37" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B38" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C38" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B39" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C39" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B40" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C40" t="s">
-        <v>89</v>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>167</v>
+      </c>
+      <c r="B41" t="s">
+        <v>166</v>
+      </c>
+      <c r="C41" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B43" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C43" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B44" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C44" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -1350,7 +1373,7 @@
         <v>30</v>
       </c>
       <c r="C45" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -1361,7 +1384,7 @@
         <v>32</v>
       </c>
       <c r="C46" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -1372,7 +1395,7 @@
         <v>34</v>
       </c>
       <c r="C47" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -1383,29 +1406,29 @@
         <v>36</v>
       </c>
       <c r="C48" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B49" t="s">
         <v>37</v>
       </c>
       <c r="C49" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
+        <v>79</v>
+      </c>
+      <c r="B51" t="s">
         <v>81</v>
       </c>
-      <c r="B51" t="s">
-        <v>83</v>
-      </c>
       <c r="C51" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -1416,7 +1439,7 @@
         <v>44</v>
       </c>
       <c r="C52" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -1427,7 +1450,7 @@
         <v>45</v>
       </c>
       <c r="C53" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -1438,7 +1461,7 @@
         <v>46</v>
       </c>
       <c r="C54" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -1449,161 +1472,172 @@
         <v>47</v>
       </c>
       <c r="C55" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B57" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C57" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B58" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C58" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C59" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C60" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C61" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B63" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C63" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B64" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C64" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B65" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C65" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B66" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C66" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B67" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C67" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B68" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C68" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B69" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C69" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B71" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C71" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C72" t="s">
-        <v>89</v>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>165</v>
+      </c>
+      <c r="B74" t="s">
+        <v>164</v>
+      </c>
+      <c r="C74" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1620,7 +1654,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1631,98 +1665,98 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>65</v>
+        <v>162</v>
       </c>
       <c r="B1" t="s">
-        <v>50</v>
+        <v>163</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" t="s">
         <v>51</v>
-      </c>
-      <c r="B2" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8" t="s">
         <v>63</v>
-      </c>
-      <c r="B8" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B10" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B12" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -1763,7 +1797,7 @@
         <v>18</v>
       </c>
       <c r="E1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1802,7 +1836,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D4" t="s">
         <v>19</v>
@@ -1853,13 +1887,13 @@
         <v>12</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D7" t="s">
         <v>20</v>
       </c>
       <c r="E7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added confirmation for test connection
</commit_message>
<xml_diff>
--- a/doc/messages.xlsx
+++ b/doc/messages.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="189">
   <si>
     <t>Error</t>
   </si>
@@ -572,6 +572,18 @@
   </si>
   <si>
     <t>ERR411</t>
+  </si>
+  <si>
+    <t>Confirm the test connection (it will save the current settings)</t>
+  </si>
+  <si>
+    <t>CONF907</t>
+  </si>
+  <si>
+    <t>ERR412</t>
+  </si>
+  <si>
+    <t>Cannot perform test connection, mandatory fields are missing in the settings window</t>
   </si>
 </sst>
 </file>
@@ -667,8 +679,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C88" totalsRowShown="0">
-  <autoFilter ref="A1:C88"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C91" totalsRowShown="0">
+  <autoFilter ref="A1:C91"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Error"/>
     <tableColumn id="2" name="Error code"/>
@@ -990,10 +1002,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C84"/>
+  <dimension ref="A1:C87"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1256,34 +1268,34 @@
         <v>86</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>68</v>
-      </c>
-      <c r="B27" t="s">
-        <v>43</v>
-      </c>
-      <c r="C27" t="s">
-        <v>170</v>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>188</v>
+      </c>
+      <c r="B26" t="s">
+        <v>187</v>
+      </c>
+      <c r="C26" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>145</v>
+        <v>68</v>
       </c>
       <c r="B28" t="s">
-        <v>146</v>
+        <v>43</v>
       </c>
       <c r="C28" t="s">
-        <v>86</v>
+        <v>170</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="B29" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="C29" t="s">
         <v>86</v>
@@ -1291,37 +1303,37 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>172</v>
+        <v>155</v>
       </c>
       <c r="B30" t="s">
-        <v>171</v>
+        <v>156</v>
+      </c>
+      <c r="C30" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>172</v>
+      </c>
+      <c r="B31" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>174</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B32" t="s">
         <v>173</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>27</v>
-      </c>
-      <c r="B33" t="s">
-        <v>49</v>
-      </c>
-      <c r="C33" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>124</v>
+        <v>27</v>
       </c>
       <c r="B34" t="s">
-        <v>119</v>
+        <v>49</v>
       </c>
       <c r="C34" t="s">
         <v>86</v>
@@ -1329,32 +1341,32 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>106</v>
+        <v>124</v>
       </c>
       <c r="B35" t="s">
-        <v>97</v>
+        <v>119</v>
       </c>
       <c r="C35" t="s">
-        <v>170</v>
+        <v>86</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="B36" t="s">
-        <v>135</v>
+        <v>97</v>
       </c>
       <c r="C36" t="s">
-        <v>86</v>
+        <v>170</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="B37" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C37" t="s">
         <v>86</v>
@@ -1362,32 +1374,32 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>133</v>
+      </c>
+      <c r="B38" t="s">
+        <v>134</v>
+      </c>
+      <c r="C38" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>158</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B39" t="s">
         <v>157</v>
       </c>
-      <c r="C38" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>179</v>
-      </c>
-      <c r="B40" t="s">
-        <v>92</v>
-      </c>
-      <c r="C40" t="s">
+      <c r="C39" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>136</v>
+        <v>179</v>
       </c>
       <c r="B41" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C41" t="s">
         <v>86</v>
@@ -1395,10 +1407,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>95</v>
+        <v>136</v>
       </c>
       <c r="B42" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C42" t="s">
         <v>86</v>
@@ -1406,32 +1418,32 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>118</v>
+        <v>95</v>
       </c>
       <c r="B43" t="s">
-        <v>117</v>
+        <v>96</v>
       </c>
       <c r="C43" t="s">
-        <v>170</v>
+        <v>86</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>154</v>
+        <v>118</v>
       </c>
       <c r="B44" t="s">
-        <v>153</v>
+        <v>117</v>
       </c>
       <c r="C44" t="s">
-        <v>86</v>
+        <v>170</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="B45" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="C45" t="s">
         <v>86</v>
@@ -1439,10 +1451,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B46" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C46" t="s">
         <v>86</v>
@@ -1450,32 +1462,32 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>166</v>
+      </c>
+      <c r="B47" t="s">
+        <v>165</v>
+      </c>
+      <c r="C47" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>177</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B48" t="s">
         <v>178</v>
       </c>
-      <c r="C47" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>102</v>
-      </c>
-      <c r="B49" t="s">
-        <v>103</v>
-      </c>
-      <c r="C49" t="s">
+      <c r="C48" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>142</v>
+        <v>102</v>
       </c>
       <c r="B50" t="s">
-        <v>143</v>
+        <v>103</v>
       </c>
       <c r="C50" t="s">
         <v>86</v>
@@ -1483,10 +1495,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>29</v>
+        <v>142</v>
       </c>
       <c r="B51" t="s">
-        <v>30</v>
+        <v>143</v>
       </c>
       <c r="C51" t="s">
         <v>86</v>
@@ -1494,10 +1506,10 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B52" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C52" t="s">
         <v>86</v>
@@ -1505,10 +1517,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B53" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C53" t="s">
         <v>86</v>
@@ -1516,10 +1528,10 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B54" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C54" t="s">
         <v>86</v>
@@ -1527,32 +1539,32 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
+        <v>35</v>
+      </c>
+      <c r="B55" t="s">
+        <v>36</v>
+      </c>
+      <c r="C55" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>61</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B56" t="s">
         <v>37</v>
       </c>
-      <c r="C55" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>78</v>
-      </c>
-      <c r="B57" t="s">
-        <v>80</v>
-      </c>
-      <c r="C57" t="s">
+      <c r="C56" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>38</v>
+        <v>78</v>
       </c>
       <c r="B58" t="s">
-        <v>44</v>
+        <v>80</v>
       </c>
       <c r="C58" t="s">
         <v>86</v>
@@ -1560,10 +1572,10 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B59" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C59" t="s">
         <v>86</v>
@@ -1571,10 +1583,10 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B60" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C60" t="s">
         <v>86</v>
@@ -1582,54 +1594,54 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
+        <v>40</v>
+      </c>
+      <c r="B61" t="s">
+        <v>46</v>
+      </c>
+      <c r="C61" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
         <v>41</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B62" t="s">
         <v>47</v>
       </c>
-      <c r="C61" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+      <c r="C62" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>94</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B64" t="s">
         <v>66</v>
       </c>
-      <c r="C63" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A64" s="5" t="s">
+      <c r="C64" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A65" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B65" t="s">
         <v>67</v>
       </c>
-      <c r="C64" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C66" t="s">
+      <c r="C65" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>148</v>
+        <v>64</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>147</v>
+        <v>65</v>
       </c>
       <c r="C67" t="s">
         <v>86</v>
@@ -1637,80 +1649,73 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C68" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="B68" s="2" t="s">
+      <c r="B69" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="C68" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="6"/>
-      <c r="B69" s="6"/>
+      <c r="C69" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="6" t="s">
-        <v>180</v>
-      </c>
-      <c r="B70" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="C70" t="s">
-        <v>86</v>
-      </c>
+      <c r="A70" s="6"/>
+      <c r="B70" s="6"/>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="B71" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="C71" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="B71" s="6" t="s">
+      <c r="B72" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C72" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>81</v>
-      </c>
-      <c r="B73" t="s">
-        <v>73</v>
-      </c>
-      <c r="C73" t="s">
-        <v>86</v>
-      </c>
+      <c r="A73" s="6"/>
+      <c r="B73" s="6"/>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>82</v>
+        <v>185</v>
       </c>
       <c r="B74" t="s">
-        <v>74</v>
+        <v>186</v>
       </c>
       <c r="C74" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>83</v>
-      </c>
-      <c r="B75" t="s">
-        <v>75</v>
-      </c>
-      <c r="C75" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B76" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="C76" t="s">
         <v>86</v>
@@ -1718,10 +1723,10 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="B77" t="s">
-        <v>105</v>
+        <v>74</v>
       </c>
       <c r="C77" t="s">
         <v>86</v>
@@ -1729,10 +1734,10 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>108</v>
+        <v>83</v>
       </c>
       <c r="B78" t="s">
-        <v>107</v>
+        <v>75</v>
       </c>
       <c r="C78" t="s">
         <v>86</v>
@@ -1740,32 +1745,43 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>109</v>
+        <v>84</v>
       </c>
       <c r="B79" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="C79" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>104</v>
+      </c>
+      <c r="B80" t="s">
+        <v>105</v>
+      </c>
+      <c r="C80" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>129</v>
+        <v>108</v>
       </c>
       <c r="B81" t="s">
-        <v>130</v>
+        <v>107</v>
       </c>
       <c r="C81" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>131</v>
+      <c r="A82" t="s">
+        <v>109</v>
+      </c>
+      <c r="B82" t="s">
+        <v>76</v>
       </c>
       <c r="C82" t="s">
         <v>86</v>
@@ -1773,12 +1789,34 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
+        <v>129</v>
+      </c>
+      <c r="B84" t="s">
+        <v>130</v>
+      </c>
+      <c r="C84" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C85" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
         <v>162</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B87" t="s">
         <v>161</v>
       </c>
-      <c r="C84" t="s">
+      <c r="C87" t="s">
         <v>86</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added new business rules based on country
</commit_message>
<xml_diff>
--- a/doc/messages.xlsx
+++ b/doc/messages.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="195">
   <si>
     <t>Error</t>
   </si>
@@ -590,6 +590,18 @@
   </si>
   <si>
     <t>The html file containing the report errors cannot be written into the folder. Either it does not exist or it is blocked by another program.</t>
+  </si>
+  <si>
+    <t>ERR809</t>
+  </si>
+  <si>
+    <t>GetAck raised an exception (with fault code)</t>
+  </si>
+  <si>
+    <t>Get ack received ACCESS_DENIED as file state</t>
+  </si>
+  <si>
+    <t>ERR810</t>
   </si>
 </sst>
 </file>
@@ -685,8 +697,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C92" totalsRowShown="0">
-  <autoFilter ref="A1:C92"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C94" totalsRowShown="0">
+  <autoFilter ref="A1:C94"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Error"/>
     <tableColumn id="2" name="Error code"/>
@@ -1008,10 +1020,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C88"/>
+  <dimension ref="A1:C90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A86" sqref="A86"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1488,34 +1500,34 @@
         <v>86</v>
       </c>
     </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>192</v>
+      </c>
+      <c r="B49" t="s">
+        <v>191</v>
+      </c>
+      <c r="C49" t="s">
+        <v>86</v>
+      </c>
+    </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>102</v>
+        <v>193</v>
       </c>
       <c r="B50" t="s">
-        <v>103</v>
+        <v>194</v>
       </c>
       <c r="C50" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>141</v>
-      </c>
-      <c r="B51" t="s">
-        <v>142</v>
-      </c>
-      <c r="C51" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="B52" t="s">
-        <v>30</v>
+        <v>103</v>
       </c>
       <c r="C52" t="s">
         <v>86</v>
@@ -1523,10 +1535,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>31</v>
+        <v>141</v>
       </c>
       <c r="B53" t="s">
-        <v>32</v>
+        <v>142</v>
       </c>
       <c r="C53" t="s">
         <v>86</v>
@@ -1534,10 +1546,10 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B54" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C54" t="s">
         <v>86</v>
@@ -1545,10 +1557,10 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B55" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C55" t="s">
         <v>86</v>
@@ -1556,43 +1568,43 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>61</v>
+        <v>33</v>
       </c>
       <c r="B56" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C56" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>35</v>
+      </c>
+      <c r="B57" t="s">
+        <v>36</v>
+      </c>
+      <c r="C57" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="B58" t="s">
-        <v>80</v>
+        <v>37</v>
       </c>
       <c r="C58" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>38</v>
-      </c>
-      <c r="B59" t="s">
-        <v>44</v>
-      </c>
-      <c r="C59" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>39</v>
+        <v>78</v>
       </c>
       <c r="B60" t="s">
-        <v>45</v>
+        <v>80</v>
       </c>
       <c r="C60" t="s">
         <v>86</v>
@@ -1600,10 +1612,10 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B61" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C61" t="s">
         <v>86</v>
@@ -1611,139 +1623,139 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B62" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C62" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>40</v>
+      </c>
+      <c r="B63" t="s">
+        <v>46</v>
+      </c>
+      <c r="C63" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
+        <v>41</v>
+      </c>
+      <c r="B64" t="s">
+        <v>47</v>
+      </c>
+      <c r="C64" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
         <v>94</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B66" t="s">
         <v>66</v>
       </c>
-      <c r="C64" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A65" s="5" t="s">
+      <c r="C66" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A67" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B67" t="s">
         <v>67</v>
       </c>
-      <c r="C65" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="C67" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="C68" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C69" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C70" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="B69" s="2" t="s">
+      <c r="B71" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="C69" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="6"/>
-      <c r="B70" s="6"/>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="6" t="s">
+      <c r="C71" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="6"/>
+      <c r="B72" s="6"/>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="B71" s="6" t="s">
+      <c r="B73" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="C71" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="6" t="s">
+      <c r="C73" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="B72" s="6" t="s">
+      <c r="B74" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="C72" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="6"/>
-      <c r="B73" s="6"/>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>184</v>
-      </c>
-      <c r="B74" t="s">
-        <v>185</v>
-      </c>
       <c r="C74" t="s">
         <v>86</v>
       </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="6"/>
+      <c r="B75" s="6"/>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>81</v>
+        <v>184</v>
       </c>
       <c r="B76" t="s">
-        <v>73</v>
+        <v>185</v>
       </c>
       <c r="C76" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>82</v>
-      </c>
-      <c r="B77" t="s">
-        <v>74</v>
-      </c>
-      <c r="C77" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B78" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C78" t="s">
         <v>86</v>
@@ -1751,10 +1763,10 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B79" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C79" t="s">
         <v>86</v>
@@ -1762,10 +1774,10 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>104</v>
+        <v>83</v>
       </c>
       <c r="B80" t="s">
-        <v>105</v>
+        <v>75</v>
       </c>
       <c r="C80" t="s">
         <v>86</v>
@@ -1773,10 +1785,10 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>108</v>
+        <v>84</v>
       </c>
       <c r="B81" t="s">
-        <v>107</v>
+        <v>85</v>
       </c>
       <c r="C81" t="s">
         <v>86</v>
@@ -1784,56 +1796,78 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B82" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="C82" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>108</v>
+      </c>
+      <c r="B83" t="s">
+        <v>107</v>
+      </c>
+      <c r="C83" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
+        <v>109</v>
+      </c>
+      <c r="B84" t="s">
+        <v>76</v>
+      </c>
+      <c r="C84" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
         <v>190</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B86" t="s">
         <v>129</v>
       </c>
-      <c r="C84" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
+      <c r="C86" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
         <v>189</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B87" t="s">
         <v>188</v>
       </c>
-      <c r="C85" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" s="1" t="s">
+      <c r="C87" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B86" s="2" t="s">
+      <c r="B88" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="C86" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
+      <c r="C88" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
         <v>161</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B90" t="s">
         <v>160</v>
       </c>
-      <c r="C88" t="s">
+      <c r="C90" t="s">
         <v>86</v>
       </c>
     </row>

</xml_diff>